<commit_message>
docs(progress/week_7): refine data analysis
Signed-off-by: Rong "Mantle" Bao <webmaster@csmantle.top>
</commit_message>
<xml_diff>
--- a/docs/progress/week_7/数据分析表.xlsx
+++ b/docs/progress/week_7/数据分析表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29504"/>
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\hdu2025_software_eng_thesis_mgmt\docs\progress\week_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\hdu2025_software_eng_thesis_mgmt\docs\progress\week_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B60F834-F0BF-42E1-943E-581C39486D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6102EDBC-57E4-4388-9D85-8AB7565B7FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="561" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="561" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据类" sheetId="9" r:id="rId1"/>
@@ -20,19 +20,61 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">数据列表!$A$1:$D$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">数据类!$A$1:$BG$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">数据项!$A$1:$J$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">数据项!$A$1:$J$61</definedName>
+    <definedName name="数据列表_开题报告状态">数据列表!$24:$24</definedName>
+    <definedName name="数据列表_所属专业">数据列表!$7:$7</definedName>
+    <definedName name="数据列表_职称">数据列表!$20:$20</definedName>
+    <definedName name="数据列表_课题状态">数据列表!$12:$12</definedName>
+    <definedName name="数据列表_课题类型">数据列表!$2:$2</definedName>
+    <definedName name="数据列表_资格审核状态">数据列表!$17:$17</definedName>
+    <definedName name="数据项_中期检查意见">数据项!$21:$21</definedName>
+    <definedName name="数据项_中期检查成绩">数据项!$22:$22</definedName>
+    <definedName name="数据项_任务书下达时间">数据项!$17:$17</definedName>
+    <definedName name="数据项_任务内容">数据项!$18:$18</definedName>
+    <definedName name="数据项_学生专业">数据项!$12:$12</definedName>
+    <definedName name="数据项_学生姓名">数据项!$11:$11</definedName>
+    <definedName name="数据项_学生学号">数据项!$10:$10</definedName>
+    <definedName name="数据项_开题报告正文">数据项!$19:$19</definedName>
+    <definedName name="数据项_开题报告状态">数据项!$20:$20</definedName>
+    <definedName name="数据项_志愿序号">数据项!$14:$14</definedName>
+    <definedName name="数据项_志愿提交时间">数据项!$16:$16</definedName>
+    <definedName name="数据项_志愿课题编号">数据项!$15:$15</definedName>
+    <definedName name="数据项_总评成绩">数据项!$26:$26</definedName>
+    <definedName name="数据项_指导教师姓名">数据项!$7:$7</definedName>
+    <definedName name="数据项_指导教师工号">数据项!$8:$8</definedName>
+    <definedName name="数据项_指导教师评分">数据项!$24:$24</definedName>
+    <definedName name="数据项_教师联系方式">数据项!$9:$9</definedName>
+    <definedName name="数据项_答辩评分">数据项!$25:$25</definedName>
+    <definedName name="数据项_论文查重率">数据项!$23:$23</definedName>
+    <definedName name="数据项_课题名称">数据项!$3:$3</definedName>
+    <definedName name="数据项_课题描述">数据项!$5:$5</definedName>
+    <definedName name="数据项_课题类型">数据项!$4:$4</definedName>
+    <definedName name="数据项_课题编号">数据项!$2:$2</definedName>
+    <definedName name="数据项_课题面向专业">数据项!$6:$6</definedName>
+    <definedName name="数据项_资格审核状态">数据项!$13:$13</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="275" uniqueCount="188">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="312" uniqueCount="180">
   <si>
     <t>序号</t>
   </si>
@@ -70,18 +112,9 @@
     <t>指导教师姓名</t>
   </si>
   <si>
-    <t>所在研究所（室、部）</t>
-  </si>
-  <si>
     <t>课题面向专业</t>
   </si>
   <si>
-    <t>教师愿意公布的联系方式</t>
-  </si>
-  <si>
-    <t>毕业设计（论文）题目</t>
-  </si>
-  <si>
     <t>数据项名称</t>
   </si>
   <si>
@@ -109,9 +142,6 @@
     <t>数值型</t>
   </si>
   <si>
-    <t>500字节</t>
-  </si>
-  <si>
     <t>数据列表取值</t>
   </si>
   <si>
@@ -131,9 +161,6 @@
   </si>
   <si>
     <t>开题报告审核通过后方可进入下一阶段</t>
-  </si>
-  <si>
-    <t>学生必须在规定时间节点前提交</t>
   </si>
   <si>
     <t>学生资格审核信息表</t>
@@ -180,9 +207,6 @@
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>教师信息</t>
-  </si>
-  <si>
     <t>课题名称</t>
   </si>
   <si>
@@ -192,107 +216,18 @@
     <t>课题描述</t>
   </si>
   <si>
-    <t>专业要求</t>
-  </si>
-  <si>
-    <t>接纳学生要求</t>
-  </si>
-  <si>
-    <t>学号</t>
-  </si>
-  <si>
-    <t>姓名</t>
-  </si>
-  <si>
-    <t>专业</t>
-  </si>
-  <si>
-    <t>班级</t>
-  </si>
-  <si>
     <t>资格审核状态</t>
   </si>
   <si>
-    <t>审核意见</t>
-  </si>
-  <si>
-    <t>审核人</t>
-  </si>
-  <si>
-    <t>学生ID</t>
-  </si>
-  <si>
-    <t>志愿序列</t>
-  </si>
-  <si>
-    <t>课题ID</t>
-  </si>
-  <si>
-    <t>提交时间</t>
-  </si>
-  <si>
-    <t>任务名称</t>
-  </si>
-  <si>
     <t>任务内容</t>
   </si>
   <si>
-    <t>进度安排</t>
-  </si>
-  <si>
-    <t>参考文献</t>
-  </si>
-  <si>
-    <t>预期成果</t>
-  </si>
-  <si>
-    <t>考核方式</t>
-  </si>
-  <si>
-    <t>报告标题</t>
-  </si>
-  <si>
-    <t>选题依据</t>
-  </si>
-  <si>
-    <t>研究方案</t>
-  </si>
-  <si>
-    <t>工作计划</t>
-  </si>
-  <si>
-    <t>指导教师审核意见</t>
-  </si>
-  <si>
-    <t>当前完成内容</t>
-  </si>
-  <si>
-    <t>存在问题</t>
-  </si>
-  <si>
-    <t>下一步计划</t>
-  </si>
-  <si>
-    <t>指导教师评定成绩</t>
-  </si>
-  <si>
     <t>指导教师评分</t>
   </si>
   <si>
-    <t>评阅教师评分</t>
-  </si>
-  <si>
     <t>答辩评分</t>
   </si>
   <si>
-    <t>学号</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
-    <t>总评成绩与等级</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
     <t>课题编号</t>
   </si>
   <si>
@@ -326,9 +261,6 @@
     <t>取值范围: [1, 3]</t>
   </si>
   <si>
-    <t>任务书下达日期</t>
-  </si>
-  <si>
     <t>日期型</t>
   </si>
   <si>
@@ -362,9 +294,6 @@
     <t>10字符</t>
   </si>
   <si>
-    <t>1, 3, 4, 7</t>
-  </si>
-  <si>
     <t>100字符</t>
   </si>
   <si>
@@ -413,15 +342,6 @@
     <t>1, 4, 5, 6, 7</t>
   </si>
   <si>
-    <t>指导教师所属的研究所或部门</t>
-  </si>
-  <si>
-    <t>根据登录账号信息自动关联</t>
-  </si>
-  <si>
-    <t>根据人事信息自动关联，可手动更新</t>
-  </si>
-  <si>
     <t>教师愿意向选定其课题的学生公开的联系方式</t>
   </si>
   <si>
@@ -470,9 +390,6 @@
     <t>选题关系确认后，由系统自动记录</t>
   </si>
   <si>
-    <t>格式: YYYY-MM-DD</t>
-  </si>
-  <si>
     <t>取值范围: [0, 100]，整数</t>
   </si>
   <si>
@@ -560,21 +477,9 @@
     <t>毕业设计开题报告</t>
   </si>
   <si>
-    <t>毕业设计中期检查表</t>
-  </si>
-  <si>
     <t>毕业设计成绩评定表</t>
   </si>
   <si>
-    <t>毕业设计课题名称</t>
-  </si>
-  <si>
-    <t>最大长度40字符</t>
-  </si>
-  <si>
-    <t>40字符</t>
-  </si>
-  <si>
     <t>讲师</t>
   </si>
   <si>
@@ -590,9 +495,6 @@
     <t>职称</t>
   </si>
   <si>
-    <t>指导教师的职称</t>
-  </si>
-  <si>
     <t>待提交</t>
   </si>
   <si>
@@ -609,15 +511,129 @@
   </si>
   <si>
     <t>打回修改</t>
+  </si>
+  <si>
+    <t>学生专业</t>
+  </si>
+  <si>
+    <t>学生学号</t>
+  </si>
+  <si>
+    <t>志愿提交时间</t>
+  </si>
+  <si>
+    <t>学生提交选题志愿的时间</t>
+  </si>
+  <si>
+    <t>任务书下达时间</t>
+  </si>
+  <si>
+    <t>提交选题志愿后，由系统自动记录</t>
+  </si>
+  <si>
+    <t>格式：YYYY-MM-DD HH:MM:SS</t>
+  </si>
+  <si>
+    <t>格式: YYYY-MM-DD HH:MM:SS</t>
+  </si>
+  <si>
+    <t>毕设任务书的具体正文内容</t>
+  </si>
+  <si>
+    <t>必填项</t>
+  </si>
+  <si>
+    <t>500字符</t>
+  </si>
+  <si>
+    <t>2000字符</t>
+  </si>
+  <si>
+    <t>志愿课题编号</t>
+  </si>
+  <si>
+    <t>学生填报选题的志愿编号</t>
+  </si>
+  <si>
+    <t>用户输入（学生）</t>
+  </si>
+  <si>
+    <t>必填，限填所有可选课题编号</t>
+  </si>
+  <si>
+    <t>取值范围：所有可选课题编号</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>答辩组对论文答辩情况的评分</t>
+  </si>
+  <si>
+    <t>用户输入（答辩组）</t>
+  </si>
+  <si>
+    <t>必填，答辩阶段由答辩组给出</t>
+  </si>
+  <si>
+    <t>取值范围：[0，100]，保留1位小数</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>混合(输入+生成)</t>
+  </si>
+  <si>
+    <t>2, 3, 5, 6, 7</t>
+  </si>
+  <si>
+    <t>开题报告正文</t>
+  </si>
+  <si>
+    <t>开题报告的正文内容</t>
+  </si>
+  <si>
+    <t>10000字符</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>中期检查意见</t>
+  </si>
+  <si>
+    <t>指导教师对学生中期进展评定的意见</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>教师必须在规定时间节点前提交</t>
+  </si>
+  <si>
+    <t>毕业设计中期检查结果表</t>
+  </si>
+  <si>
+    <t>指导教师工号</t>
+  </si>
+  <si>
+    <t>指导教师的工号</t>
+  </si>
+  <si>
+    <t>教师公开联系方式</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 5, 6, 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="29">
     <font>
-      <sz val="12"/>
+      <sz val="10.5"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -773,6 +789,26 @@
     </font>
     <font>
       <sz val="10.5"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10.5"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10.5"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -942,7 +978,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="12">
     <border>
       <start/>
       <end/>
@@ -960,30 +996,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start style="thin">
-        <color auto="1"/>
-      </start>
-      <end style="thin">
-        <color auto="1"/>
-      </end>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <start style="thin">
-        <color auto="1"/>
-      </start>
-      <end style="thin">
-        <color auto="1"/>
-      </end>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1109,61 +1121,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <start/>
-      <end/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start/>
-      <end/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start/>
-      <end style="thin">
-        <color auto="1"/>
-      </end>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start style="thin">
-        <color auto="1"/>
-      </start>
-      <end/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <start/>
-      <end style="thin">
-        <color indexed="64"/>
-      </end>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -1171,7 +1130,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1195,7 +1154,7 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1243,13 +1202,13 @@
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1271,10 +1230,10 @@
     <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1283,10 +1242,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
@@ -1299,11 +1258,13 @@
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1328,73 +1289,73 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="25" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1403,11 +1364,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="50">
     <cellStyle name="20% - 着色 1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="20% - 着色 2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
     <cellStyle name="20% - 着色 3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
@@ -1427,7 +1385,9 @@
     <cellStyle name="60% - 着色 4 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
     <cellStyle name="60% - 着色 5 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="60% - 着色 6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="好 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
     <cellStyle name="差 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
     <cellStyle name="常规 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
@@ -1758,103 +1718,104 @@
   </sheetPr>
   <dimension ref="A1:BG8"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K6" sqref="A1:BG8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="3"/>
-    <col min="2" max="2" width="23.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.58203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.4140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.58203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10.58203125" style="3" customWidth="1"/>
-    <col min="8" max="9" width="10.58203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="18.9140625" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="18.5" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="13.1640625" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="21.6640625" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="58" width="10.58203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="10.58203125" style="3" customWidth="1"/>
-    <col min="60" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="9.08984375" style="3"/>
+    <col min="2" max="2" width="23.36328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.90625" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="13.81640625" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="19" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="18.54296875" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="20.54296875" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="21.7265625" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="58" width="10.6328125" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="10.6328125" style="3" customWidth="1"/>
+    <col min="60" max="16384" width="9.08984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="19" customFormat="1" ht="22" customHeight="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:59" s="25" customFormat="1" ht="22" customHeight="1">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
-      <c r="BB1" s="18"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="18"/>
-      <c r="BE1" s="18"/>
-      <c r="BF1" s="18"/>
-      <c r="BG1" s="17" t="s">
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="28"/>
+      <c r="AQ1" s="28"/>
+      <c r="AR1" s="28"/>
+      <c r="AS1" s="28"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="28"/>
+      <c r="AX1" s="28"/>
+      <c r="AY1" s="28"/>
+      <c r="AZ1" s="28"/>
+      <c r="BA1" s="28"/>
+      <c r="BB1" s="28"/>
+      <c r="BC1" s="28"/>
+      <c r="BD1" s="28"/>
+      <c r="BE1" s="28"/>
+      <c r="BF1" s="28"/>
+      <c r="BG1" s="24" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1863,13 +1824,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>9</v>
@@ -1877,26 +1838,26 @@
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>15</v>
+      <c r="J2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -1950,13 +1911,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>9</v>
@@ -1964,27 +1925,21 @@
       <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="G3" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -2037,13 +1992,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>9</v>
@@ -2051,19 +2006,19 @@
       <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="K4" s="8"/>
+      <c r="G4" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="K4" s="2"/>
       <c r="L4" s="8"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -2117,13 +2072,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>9</v>
@@ -2131,24 +2086,18 @@
       <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="G5" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -2202,13 +2151,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
@@ -2216,21 +2165,20 @@
       <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="G6" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -2284,13 +2232,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>174</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
@@ -2298,17 +2246,20 @@
       <c r="F7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>76</v>
+      <c r="G7" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -2364,38 +2315,44 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="G8" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -2453,6 +2410,42 @@
       <formula1>"系统存储,临时生成"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J2" location="数据项_课题名称" display="课题名称" xr:uid="{AF9D8032-277F-4698-937E-A15063A0AFCD}"/>
+    <hyperlink ref="K2" location="数据项_课题类型" display="课题类型" xr:uid="{022D4CE3-CA0A-4216-A591-7375C5950CD4}"/>
+    <hyperlink ref="L2" location="数据项_课题描述" display="课题描述" xr:uid="{BD1ED4E7-0A3D-447A-AF0D-1C9F80F3B0A5}"/>
+    <hyperlink ref="M2" location="数据项_课题面向专业" display="课题面向专业" xr:uid="{685966FA-6187-435D-85DA-42C3C648E854}"/>
+    <hyperlink ref="G3" location="数据项_学生学号" display="学生学号" xr:uid="{ADBA4252-92FD-429F-9DEB-57751147E07C}"/>
+    <hyperlink ref="H3" location="数据项_学生姓名" display="学生姓名" xr:uid="{7B290423-EBB3-49E0-962F-B4056C3AC486}"/>
+    <hyperlink ref="I3" location="数据项_学生专业" display="学生专业" xr:uid="{D53F6954-C4CF-4FB6-89A6-D0D3B64806ED}"/>
+    <hyperlink ref="J3" location="数据项_资格审核状态" display="资格审核状态" xr:uid="{B0A49BEF-A094-471F-BE50-869891DCF2DF}"/>
+    <hyperlink ref="H4" location="数据项_志愿序号" display="志愿序号" xr:uid="{46ACFDA1-71A3-4B45-9AE4-AF07AE2C4F2F}"/>
+    <hyperlink ref="I4" location="数据项_志愿课题编号" display="志愿课题编号" xr:uid="{D159D452-36A9-4E30-8925-CA0D956E1D9E}"/>
+    <hyperlink ref="J4" location="数据项_志愿提交时间" display="志愿提交时间" xr:uid="{7486B97D-2CAC-4449-9646-E88F9308E5CC}"/>
+    <hyperlink ref="G4" location="数据项_学生学号" display="学生学号" xr:uid="{7D8D1961-6919-4D80-8647-0CE7904A1CF3}"/>
+    <hyperlink ref="G6" location="数据项_学生学号" display="学生学号" xr:uid="{17F3D1EC-8E13-4C7B-BFA7-1C452F275EB6}"/>
+    <hyperlink ref="G7" location="数据项_学生学号" display="学生学号" xr:uid="{EAAB3E53-B011-49DC-B134-19ECDDDA7B83}"/>
+    <hyperlink ref="G8" location="数据项_学生学号" display="学生学号" xr:uid="{A784EDFF-99EB-40AB-AEC1-F7614055EC90}"/>
+    <hyperlink ref="H5" location="数据项_任务书下达时间" display="任务书下达时间" xr:uid="{07F62756-C8C4-435D-BB10-36387FDFB980}"/>
+    <hyperlink ref="I5" location="数据项_任务内容" display="任务内容" xr:uid="{7AFC92F3-B583-43B1-8A3D-7AF4C4D4B6F6}"/>
+    <hyperlink ref="J6" location="数据项_开题报告状态" display="指导教师审核意见" xr:uid="{21EAD18C-8B90-44BB-8C6B-1691C2A10341}"/>
+    <hyperlink ref="I6" location="数据项_开题报告正文" display="开题报告正文" xr:uid="{FF2C5D0E-1E1A-453F-B926-AFA57EB7E47B}"/>
+    <hyperlink ref="K7" location="数据项_中期检查成绩" display="中期检查成绩" xr:uid="{FF080BBC-E74E-4F1C-8372-67EC312380A1}"/>
+    <hyperlink ref="J8" location="数据项_论文查重率" display="论文查重率" xr:uid="{8091E1C4-3B01-45CF-B410-D41A215E1F12}"/>
+    <hyperlink ref="K8" location="数据项_指导教师评分" display="指导教师评分" xr:uid="{AA029905-921B-496A-902D-B5E163800132}"/>
+    <hyperlink ref="L8" location="数据项_答辩评分" display="答辩评分" xr:uid="{1018FD73-6D24-4542-A2F1-3BE5FEFFDBD2}"/>
+    <hyperlink ref="M8" location="数据项_总评成绩" display="总评成绩" xr:uid="{498AF98A-D45F-4586-B32B-27C4CD50E813}"/>
+    <hyperlink ref="J7" location="数据项_中期检查意见" display="中期检查意见" xr:uid="{B18746CB-2073-4395-8B9F-893E2A774526}"/>
+    <hyperlink ref="G2" location="数据项_指导教师姓名" display="教师姓名" xr:uid="{974A1C37-7DFA-46BE-A46A-DF386FB3A6AF}"/>
+    <hyperlink ref="H2" location="数据项_指导教师工号" display="教师工号" xr:uid="{6916FCE9-9FB9-478A-8EAF-BDCBF31A9AA2}"/>
+    <hyperlink ref="I7" location="数据项_指导教师工号" display="教师工号" xr:uid="{A9F936F4-43A9-4FCA-8882-638C0D82820C}"/>
+    <hyperlink ref="I8" location="数据项_指导教师工号" display="指导教师工号" xr:uid="{70971C7D-E632-4B03-B38C-4826C16DCA32}"/>
+    <hyperlink ref="G5" location="数据项_课题编号" display="课题编号" xr:uid="{2FFB2B5A-ABE9-4E92-AE05-09E4119B4631}"/>
+    <hyperlink ref="H6" location="数据项_课题编号" display="课题编号" xr:uid="{637F0D74-09AB-44A6-81FD-CA40B143DDE4}"/>
+    <hyperlink ref="H7" location="数据项_课题编号" display="课题编号" xr:uid="{E1329DAB-8725-4AB1-BEFD-474144203AB5}"/>
+    <hyperlink ref="H8" location="数据项_课题编号" display="课题编号" xr:uid="{2C3A88D9-1E7C-4206-9C09-4A873E144687}"/>
+    <hyperlink ref="I2" location="数据项_课题编号" display="课题编号" xr:uid="{D1EBA833-DAE9-4B4A-8856-D3FE3B221CBC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
@@ -2464,56 +2457,56 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="24"/>
-    <col min="2" max="2" width="21.83203125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="37.5" style="24" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="26" customWidth="1"/>
-    <col min="6" max="6" width="36.75" style="24" customWidth="1"/>
-    <col min="7" max="7" width="37.58203125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="26" customWidth="1"/>
-    <col min="9" max="9" width="25.4140625" style="27" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="24" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="24"/>
+    <col min="1" max="1" width="9.08984375" style="1"/>
+    <col min="2" max="2" width="21.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="36.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37.6328125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.453125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="16.36328125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="25" customFormat="1" ht="22" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:10" s="23" customFormat="1" ht="22" customHeight="1">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="I1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2522,28 +2515,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>105</v>
+        <v>66</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>179</v>
       </c>
       <c r="J2" s="7"/>
     </row>
@@ -2552,28 +2545,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>173</v>
+        <v>40</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>107</v>
+        <v>50</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="J3" s="7"/>
     </row>
@@ -2582,28 +2575,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>139</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>111</v>
+        <v>72</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>74</v>
       </c>
       <c r="J4" s="7"/>
     </row>
@@ -2612,25 +2605,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>25</v>
+        <v>76</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>152</v>
       </c>
       <c r="I5" s="21">
         <v>1</v>
@@ -2642,31 +2635,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>22</v>
+        <v>139</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>116</v>
+        <v>72</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>79</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13.5" customHeight="1">
@@ -2677,25 +2670,25 @@
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>121</v>
+        <v>82</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>84</v>
       </c>
       <c r="J7" s="7"/>
     </row>
@@ -2703,29 +2696,29 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>122</v>
+      <c r="B8" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>177</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="I8" s="21">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>84</v>
       </c>
       <c r="J8" s="7"/>
     </row>
@@ -2733,26 +2726,26 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>180</v>
+      <c r="B9" s="26" t="s">
+        <v>178</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>181</v>
+        <v>85</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>110</v>
+        <v>86</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="I9" s="21">
         <v>1</v>
@@ -2764,28 +2757,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I10" s="21">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>166</v>
       </c>
       <c r="J10" s="7"/>
     </row>
@@ -2794,28 +2787,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>131</v>
+        <v>94</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="J11" s="7"/>
     </row>
@@ -2824,28 +2817,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>131</v>
+        <v>94</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="J12" s="7"/>
     </row>
@@ -2854,28 +2847,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>22</v>
+        <v>140</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>131</v>
+        <v>96</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="21">
+        <v>3</v>
       </c>
       <c r="J13" s="7"/>
     </row>
@@ -2884,25 +2877,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>110</v>
+        <v>98</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="I14" s="21">
         <v>3</v>
@@ -2914,28 +2907,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I15" s="21">
-        <v>3</v>
+        <v>157</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>159</v>
       </c>
       <c r="J15" s="7"/>
     </row>
@@ -2944,28 +2937,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>110</v>
+        <v>147</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="I16" s="21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J16" s="7"/>
     </row>
@@ -2974,28 +2967,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>184</v>
+        <v>99</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>110</v>
+        <v>100</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="I17" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J17" s="7"/>
     </row>
@@ -3004,28 +2997,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>110</v>
+        <v>151</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>153</v>
       </c>
       <c r="I18" s="21">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J18" s="7"/>
     </row>
@@ -3034,28 +3027,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I19" s="21">
-        <v>7</v>
+        <v>151</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="J19" s="7"/>
     </row>
@@ -3064,28 +3057,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>24</v>
+        <v>139</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>110</v>
+        <v>59</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="I20" s="21">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J20" s="7"/>
     </row>
@@ -3094,153 +3087,310 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>99</v>
+        <v>172</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H22" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" s="21">
+        <v>6</v>
+      </c>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="21">
+        <v>7</v>
+      </c>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="21">
+        <v>7</v>
+      </c>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="I21" s="21">
+      <c r="G26" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="21">
         <v>7</v>
       </c>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="26"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="26"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="26"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="26"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="26"/>
+      <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="26"/>
-      <c r="I27" s="28"/>
+      <c r="A27" s="13"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="26"/>
+      <c r="A28" s="13"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="26"/>
+      <c r="A29" s="13"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="26"/>
+      <c r="A30" s="13"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="26"/>
-      <c r="I31" s="28"/>
+      <c r="A31" s="13"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="26"/>
+      <c r="A32" s="13"/>
+      <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="26"/>
+      <c r="A33" s="13"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="26"/>
+      <c r="A34" s="13"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="26"/>
+      <c r="A35" s="13"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="26"/>
+      <c r="A36" s="13"/>
+      <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="26"/>
+      <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="26"/>
+      <c r="A38" s="13"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="26"/>
+      <c r="A39" s="13"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="26"/>
+      <c r="A40" s="13"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="26"/>
+      <c r="A41" s="13"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="26"/>
-      <c r="B42" s="29"/>
-      <c r="I42" s="30"/>
+      <c r="A42" s="13"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="26"/>
+      <c r="A43" s="13"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="26"/>
-      <c r="I44" s="28"/>
+      <c r="A44" s="13"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="26"/>
+      <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="26"/>
+      <c r="A46" s="13"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="26"/>
-      <c r="I47" s="28"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+      <c r="I47" s="17"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="26"/>
+      <c r="A48" s="13"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="26"/>
+      <c r="A49" s="13"/>
+      <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="26"/>
+      <c r="A50" s="13"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="26"/>
+      <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="26"/>
-      <c r="B52" s="29"/>
-      <c r="I52" s="30"/>
+      <c r="A52" s="13"/>
+      <c r="I52" s="15"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="26"/>
+      <c r="A53" s="13"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="26"/>
-      <c r="I54" s="28"/>
+      <c r="A54" s="13"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="26"/>
-      <c r="I55" s="30"/>
+      <c r="A55" s="13"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="26"/>
+      <c r="A56" s="13"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+      <c r="I57" s="17"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="13"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="13"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="13"/>
+      <c r="I60" s="17"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="24" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22:D56" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D27:D61" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"外部系统,用户输入,系统生成"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E6" location="数据列表_所属专业" display="列表型" xr:uid="{3F1D0D07-8EBB-4B8E-8F9A-C54DBAE829C9}"/>
+    <hyperlink ref="E12" location="数据列表_所属专业" display="列表型" xr:uid="{BC39B89A-766D-4439-85A4-4C961D0DB760}"/>
+    <hyperlink ref="E13" location="数据列表_资格审核状态" display="列表型" xr:uid="{D56FB2D9-C358-46DE-9943-52DB79D5DF62}"/>
+    <hyperlink ref="E20" location="数据列表_开题报告状态" display="列表型" xr:uid="{E0C86225-26DE-44DE-848D-5C8CBE156BBB}"/>
+    <hyperlink ref="E4" location="数据列表_课题类型" display="列表型" xr:uid="{6D65A606-9FF2-4875-98AF-75F674617435}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
@@ -3254,30 +3404,29 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="16.58203125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="31.5" style="24" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="24"/>
-    <col min="5" max="16384" width="9" style="24"/>
+    <col min="1" max="1" width="4.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="25" customFormat="1" ht="15">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:4" s="12" customFormat="1" ht="15">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3286,10 +3435,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -3297,7 +3446,7 @@
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
       <c r="C3" s="7" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -3305,7 +3454,7 @@
       <c r="A4" s="31"/>
       <c r="B4" s="32"/>
       <c r="C4" s="7" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -3313,7 +3462,7 @@
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="C5" s="7" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -3321,7 +3470,7 @@
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
       <c r="C6" s="7" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="D6" s="7"/>
     </row>
@@ -3330,10 +3479,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -3341,7 +3490,7 @@
       <c r="A8" s="31"/>
       <c r="B8" s="32"/>
       <c r="C8" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -3349,7 +3498,7 @@
       <c r="A9" s="31"/>
       <c r="B9" s="32"/>
       <c r="C9" s="7" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -3357,7 +3506,7 @@
       <c r="A10" s="31"/>
       <c r="B10" s="32"/>
       <c r="C10" s="7" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="D10" s="7"/>
     </row>
@@ -3365,7 +3514,7 @@
       <c r="A11" s="31"/>
       <c r="B11" s="32"/>
       <c r="C11" s="7" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="D11" s="7"/>
     </row>
@@ -3374,10 +3523,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="D12" s="7"/>
     </row>
@@ -3385,7 +3534,7 @@
       <c r="A13" s="31"/>
       <c r="B13" s="32"/>
       <c r="C13" s="7" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="D13" s="7"/>
     </row>
@@ -3393,7 +3542,7 @@
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="7" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -3401,7 +3550,7 @@
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
       <c r="C15" s="7" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="D15" s="7"/>
     </row>
@@ -3409,7 +3558,7 @@
       <c r="A16" s="31"/>
       <c r="B16" s="32"/>
       <c r="C16" s="7" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="D16" s="7"/>
     </row>
@@ -3418,10 +3567,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="D17" s="7"/>
     </row>
@@ -3429,7 +3578,7 @@
       <c r="A18" s="31"/>
       <c r="B18" s="32"/>
       <c r="C18" s="7" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="D18" s="7"/>
     </row>
@@ -3437,96 +3586,96 @@
       <c r="A19" s="31"/>
       <c r="B19" s="32"/>
       <c r="C19" s="7" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="33">
+      <c r="A20" s="30">
         <v>5</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>180</v>
+      <c r="B20" s="29" t="s">
+        <v>135</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="33"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="2" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="33"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="2" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="33"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="2" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="33">
+      <c r="A24" s="30">
         <v>6</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>183</v>
+      <c r="B24" s="29" t="s">
+        <v>137</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>182</v>
+        <v>136</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="33"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="2" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="33"/>
-      <c r="B26" s="23"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="2" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="33"/>
-      <c r="B27" s="23"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="2" t="s">
-        <v>187</v>
+        <v>141</v>
       </c>
       <c r="D27" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>